<commit_message>
Fixed construction partner bugg was misisng one of the columns
</commit_message>
<xml_diff>
--- a/backend/test_output/Time-Card-2026-02-09-2026-02-15.xlsx
+++ b/backend/test_output/Time-Card-2026-02-09-2026-02-15.xlsx
@@ -6808,7 +6808,7 @@
         <v>38</v>
       </c>
       <c r="D197" s="4" t="s">
-        <v>87</v>
+        <v>19</v>
       </c>
       <c r="E197" s="2" t="s">
         <v>20</v>
@@ -10901,7 +10901,7 @@
         <v>38</v>
       </c>
       <c r="D332" s="4" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="E332" s="2" t="s">
         <v>20</v>
@@ -10939,7 +10939,7 @@
         <v>38</v>
       </c>
       <c r="D333" s="4" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="E333" s="2" t="s">
         <v>20</v>
@@ -10977,7 +10977,7 @@
         <v>42</v>
       </c>
       <c r="D334" s="4" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="E334" s="2" t="s">
         <v>20</v>
@@ -11015,7 +11015,7 @@
         <v>45</v>
       </c>
       <c r="D335" s="4" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="E335" s="2" t="s">
         <v>20</v>

</xml_diff>